<commit_message>
reorganize Ar4 and Ar3
</commit_message>
<xml_diff>
--- a/diagram/Ar2_diagram.xlsx
+++ b/diagram/Ar2_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Agiat_Ikazinat\Agiat_Ikazinat\diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1681E178-73B7-44F0-9DFD-3A18F79E72F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE997BA9-BCA9-43F8-90DF-AFA8824E8274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{252522C9-A19E-488B-90A9-38290CEECCCA}"/>
+    <workbookView xWindow="31350" yWindow="2100" windowWidth="21600" windowHeight="11235" xr2:uid="{252522C9-A19E-488B-90A9-38290CEECCCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>left_side_ankle</t>
   </si>
@@ -83,36 +83,9 @@
     <t>in2</t>
   </si>
   <si>
-    <t>M1</t>
-  </si>
-  <si>
-    <t>Num</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>right_shoulder_z</t>
-  </si>
-  <si>
-    <t>right_bicept</t>
-  </si>
-  <si>
-    <t>right_shoulder_y</t>
-  </si>
-  <si>
-    <t>right_shoulder_x</t>
-  </si>
-  <si>
-    <t>M4</t>
-  </si>
-  <si>
-    <t>M3</t>
-  </si>
-  <si>
-    <t>M2</t>
-  </si>
-  <si>
     <t>Degree (A)</t>
   </si>
   <si>
@@ -126,6 +99,33 @@
   </si>
   <si>
     <t>Mid</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Dir</t>
+  </si>
+  <si>
+    <t>Dir2</t>
+  </si>
+  <si>
+    <t>side_eye</t>
+  </si>
+  <si>
+    <t>up_eye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">head </t>
+  </si>
+  <si>
+    <t>side_neck</t>
+  </si>
+  <si>
+    <t>mouth</t>
+  </si>
+  <si>
+    <t>neck</t>
   </si>
 </sst>
 </file>
@@ -198,15 +198,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB51C1AA-5102-4CF8-A383-028DC3363D5A}" name="right_arm" displayName="right_arm" ref="J1:O5" totalsRowShown="0">
-  <autoFilter ref="J1:O5" xr:uid="{DB51C1AA-5102-4CF8-A383-028DC3363D5A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2BBDBEF5-4564-402E-845F-CF48BCC33927}" name="head" displayName="head" ref="J1:O7" totalsRowShown="0">
+  <autoFilter ref="J1:O7" xr:uid="{2BBDBEF5-4564-402E-845F-CF48BCC33927}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2EBA66A4-8D40-4FE5-9648-A613246E5A9B}" name="Name"/>
-    <tableColumn id="2" xr3:uid="{411CB8E4-CA1F-426E-8C6C-43227131EEEA}" name="Num"/>
-    <tableColumn id="3" xr3:uid="{B3D7AF98-F3BC-4209-B082-A64C336BDBA5}" name="Degree (A)"/>
-    <tableColumn id="4" xr3:uid="{79C796FB-3A81-4794-ACDA-ECE734D9FC51}" name="Min"/>
-    <tableColumn id="5" xr3:uid="{FEAABB4A-8E81-4CE9-B1B0-CB56B9C930EB}" name="Mid"/>
-    <tableColumn id="6" xr3:uid="{98690D28-E894-441A-8205-1ED11065078C}" name="Max"/>
+    <tableColumn id="1" xr3:uid="{3E6B4BAB-713A-40A2-9D1C-1883AD403F5D}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{0485B7B0-530B-484D-8AB1-9DE9EBAB542D}" name="Pin"/>
+    <tableColumn id="3" xr3:uid="{2A89E806-F806-4904-B085-3AB169BC341F}" name="Min"/>
+    <tableColumn id="4" xr3:uid="{52B9B740-FF2F-41F6-8C44-FF74EFEC71FA}" name="Dir"/>
+    <tableColumn id="5" xr3:uid="{32A97087-5479-410E-AA4C-3556750916AB}" name="Max"/>
+    <tableColumn id="6" xr3:uid="{665EC0B8-DA88-48D0-8402-9B2032163416}" name="Dir2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -532,7 +532,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,7 +545,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -557,34 +557,34 @@
         <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>25</v>
-      </c>
       <c r="M1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="O1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -604,13 +604,10 @@
         <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="K2">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -630,13 +627,10 @@
         <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" t="s">
         <v>24</v>
       </c>
-      <c r="L3">
-        <v>14</v>
+      <c r="K3">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -656,13 +650,10 @@
         <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4">
-        <v>13</v>
+        <v>28</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -682,13 +673,10 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5">
-        <v>6</v>
+        <v>25</v>
+      </c>
+      <c r="K5">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -707,6 +695,12 @@
       <c r="E6">
         <v>9</v>
       </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -723,6 +717,12 @@
       </c>
       <c r="E7">
         <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>